<commit_message>
switched to usb c from battery
</commit_message>
<xml_diff>
--- a/Hardware/LED_Matrix_2-0_BOM.xlsx
+++ b/Hardware/LED_Matrix_2-0_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eleanortaylor/Documents/GitHub/LED_Matrix/Hardware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ellie\Documents\GitHub\LED_Matrix\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F67A644-2444-2540-9AE3-23604A1F7BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F75186F-8756-4A9B-9FF4-4898F76BA9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="500" windowWidth="20280" windowHeight="17500" xr2:uid="{CBCE60BC-0067-4A82-873C-C47F583079C9}"/>
+    <workbookView xWindow="2710" yWindow="3800" windowWidth="28800" windowHeight="15460" xr2:uid="{CBCE60BC-0067-4A82-873C-C47F583079C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Part number</t>
   </si>
@@ -179,19 +179,37 @@
     <t>2721-LDI1117-05HTR-ND</t>
   </si>
   <si>
-    <t>SS-52400-003</t>
-  </si>
-  <si>
-    <t>380-SS-52400-003CT-ND</t>
-  </si>
-  <si>
-    <t>Stewart Connector</t>
-  </si>
-  <si>
     <t>USB-C</t>
   </si>
   <si>
     <t>USB-C receptable for power</t>
+  </si>
+  <si>
+    <t>UJC-HP-3-SMT-TR</t>
+  </si>
+  <si>
+    <t>CUI Devices</t>
+  </si>
+  <si>
+    <t>2223-UJC-HP-3-SMT-CT-ND</t>
+  </si>
+  <si>
+    <t>CRCW08055K10FKEAHP</t>
+  </si>
+  <si>
+    <t>Rx</t>
+  </si>
+  <si>
+    <t>5.1kOhm</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>541-CRCW08055K10FKEAHPCT-ND</t>
+  </si>
+  <si>
+    <t>USB-C CC resistors</t>
   </si>
 </sst>
 </file>
@@ -336,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -365,64 +383,67 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -740,29 +761,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD9514A-9B29-435C-BF48-54525C97080F}">
-  <dimension ref="B2:N11"/>
+  <dimension ref="B2:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.83203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="23.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.81640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.81640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.6328125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
@@ -770,7 +791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14" ht="58" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -811,18 +832,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="11">
         <v>256</v>
       </c>
-      <c r="E4" s="15">
-        <f t="shared" ref="E4:E10" si="0">D4*$C$2</f>
+      <c r="E4" s="11">
+        <f t="shared" ref="E4:E11" si="0">D4*$C$2</f>
         <v>768</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -842,19 +863,19 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="L4" s="5">
-        <f t="shared" ref="L4:L10" si="1">D4*K4</f>
+        <f t="shared" ref="L4:L11" si="1">D4*K4</f>
         <v>148.47999999999999</v>
       </c>
       <c r="M4" s="5">
         <f>K4*E4</f>
         <v>445.43999999999994</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5" s="13" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -873,7 +894,7 @@
       <c r="G5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="14" t="s">
         <v>29</v>
       </c>
       <c r="I5" s="8" t="s">
@@ -890,24 +911,24 @@
         <v>25.6</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" ref="M5:M10" si="2">K5*E5</f>
+        <f t="shared" ref="M5:M11" si="2">K5*E5</f>
         <v>76.800000000000011</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="N5" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="B6" s="20" t="s">
+    <row r="6" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="17">
         <v>1</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -935,12 +956,12 @@
         <f t="shared" si="2"/>
         <v>1.56</v>
       </c>
-      <c r="N6" s="22" t="s">
+      <c r="N6" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="B7" s="17" t="s">
+    <row r="7" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -979,150 +1000,194 @@
         <f>K7*E7</f>
         <v>1.53</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="N7" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="B8" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="21" t="s">
+    <row r="8" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="17">
         <v>1</v>
       </c>
-      <c r="E8" s="21">
-        <f t="shared" ref="E8" si="3">D8*$C$2</f>
+      <c r="E8" s="17">
+        <f t="shared" ref="E8:E9" si="3">D8*$C$2</f>
         <v>3</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="J8" s="9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="K8" s="6">
-        <v>1.51</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" ref="L8" si="4">K8*D8</f>
-        <v>1.51</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="M8" s="6">
-        <f t="shared" ref="M8" si="5">K8*E8</f>
-        <v>4.53</v>
-      </c>
-      <c r="N8" s="22" t="s">
+        <f t="shared" ref="M8:M9" si="5">K8*E8</f>
+        <v>3.4799999999999995</v>
+      </c>
+      <c r="N8" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="24">
+    <row r="9" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="21">
+        <v>2</v>
+      </c>
+      <c r="E9" s="21">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="L9" s="24">
+        <f>K9*D9</f>
+        <v>0.46</v>
+      </c>
+      <c r="M9" s="24">
+        <f t="shared" si="5"/>
+        <v>1.3800000000000001</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B10" s="16">
         <v>22122044</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C10" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D10" s="17">
         <v>1</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E10" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K10" s="6">
         <v>1.28</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L10" s="6">
         <f t="shared" si="1"/>
         <v>1.28</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M10" s="6">
         <f t="shared" si="2"/>
         <v>3.84</v>
       </c>
-      <c r="N9" s="26" t="s">
+      <c r="N10" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="B10" s="27">
+    <row r="11" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="26">
         <v>2177961041</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D11" s="27">
         <v>1</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E11" s="27">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F11" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G11" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H11" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I11" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J11" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K11" s="29">
         <v>2.87</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L11" s="29">
         <f t="shared" si="1"/>
         <v>2.87</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M11" s="29">
         <f t="shared" si="2"/>
         <v>8.61</v>
       </c>
-      <c r="N10" s="29" t="s">
+      <c r="N11" s="30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L11" s="2">
-        <f>SUM(L4:L10)</f>
-        <v>180.76999999999998</v>
-      </c>
-      <c r="M11" s="2">
-        <f>L11*$C$2</f>
-        <v>542.30999999999995</v>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="L12" s="2">
+        <f>SUM(L4:L11)</f>
+        <v>180.88</v>
+      </c>
+      <c r="M12" s="2">
+        <f>L12*$C$2</f>
+        <v>542.64</v>
       </c>
     </row>
   </sheetData>
@@ -1131,16 +1196,34 @@
     <hyperlink ref="B4" r:id="rId1" xr:uid="{3A0E0B2C-17EE-3D41-96E9-F139CB8A2E54}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{9999CBF9-0CDD-4B48-B955-7479237F2071}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{6D999CED-9711-4640-A005-827337416F33}"/>
-    <hyperlink ref="B9" r:id="rId4" display="https://www.digikey.com/en/products/detail/molex/0022122044/172037?s=N4IgTCBcDaIOoFkwHYCMBmAtAOQCIgF0BfIA" xr:uid="{7437B1C3-056F-0144-ABD4-205DC0CF3893}"/>
-    <hyperlink ref="B10" r:id="rId5" display="https://www.digikey.com/en/products/detail/molex/2177961041/14638035?s=N4IgTCBcDaIJwAYEFowEYDsG4DY0IBY1kA5AERAF0BfIA" xr:uid="{D06D4DCF-3FAD-A643-A76D-087102DD2020}"/>
+    <hyperlink ref="B10" r:id="rId4" display="https://www.digikey.com/en/products/detail/molex/0022122044/172037?s=N4IgTCBcDaIOoFkwHYCMBmAtAOQCIgF0BfIA" xr:uid="{7437B1C3-056F-0144-ABD4-205DC0CF3893}"/>
+    <hyperlink ref="B11" r:id="rId5" display="https://www.digikey.com/en/products/detail/molex/2177961041/14638035?s=N4IgTCBcDaIJwAYEFowEYDsG4DY0IBY1kA5AERAF0BfIA" xr:uid="{D06D4DCF-3FAD-A643-A76D-087102DD2020}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{9592E701-99FA-1B45-BF3D-975C7A1DA5D3}"/>
     <hyperlink ref="B8" r:id="rId7" xr:uid="{E2A5498C-D55C-FA4D-B8F4-F48B72971313}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{6AE1B05E-E8D8-4CC5-93EF-48089028ABE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ba1fd6c3-18a5-4ad5-8874-cc8651459af8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100502A07BBE43C3E4CA597A0A715DE62F0" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ef1ef2518dbd8baba4018934b602a0f9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ba1fd6c3-18a5-4ad5-8874-cc8651459af8" xmlns:ns4="a68b5875-a714-48fe-ba43-532dbf3c5e2c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="47a0e7dd0dc87d993f33ac560f56e359" ns3:_="" ns4:_="">
     <xsd:import namespace="ba1fd6c3-18a5-4ad5-8874-cc8651459af8"/>
@@ -1361,38 +1444,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ba1fd6c3-18a5-4ad5-8874-cc8651459af8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EE7C584-7962-4C7B-8A56-C0162DDCE136}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23CEE53E-8C79-44C3-9A5B-668821A655FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ba1fd6c3-18a5-4ad5-8874-cc8651459af8"/>
-    <ds:schemaRef ds:uri="a68b5875-a714-48fe-ba43-532dbf3c5e2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1415,9 +1470,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23CEE53E-8C79-44C3-9A5B-668821A655FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EE7C584-7962-4C7B-8A56-C0162DDCE136}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ba1fd6c3-18a5-4ad5-8874-cc8651459af8"/>
+    <ds:schemaRef ds:uri="a68b5875-a714-48fe-ba43-532dbf3c5e2c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refilled zones, added items to BOM
</commit_message>
<xml_diff>
--- a/Hardware/LED_Matrix_2-0_BOM.xlsx
+++ b/Hardware/LED_Matrix_2-0_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ellie\Documents\GitHub\LED_Matrix\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eleanortaylor/Documents/GitHub/LED_Matrix/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F75186F-8756-4A9B-9FF4-4898F76BA9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CF33BE-6A15-0145-855F-1A42D7D4D261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2710" yWindow="3800" windowWidth="28800" windowHeight="15460" xr2:uid="{CBCE60BC-0067-4A82-873C-C47F583079C9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CBCE60BC-0067-4A82-873C-C47F583079C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>Part number</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Size</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -167,18 +164,6 @@
     <t>Ext. Quantity</t>
   </si>
   <si>
-    <t>LDI1117-05H</t>
-  </si>
-  <si>
-    <t>Voltage regulator to lmit VDD to 5V</t>
-  </si>
-  <si>
-    <t>Diotec Semiconductor</t>
-  </si>
-  <si>
-    <t>2721-LDI1117-05HTR-ND</t>
-  </si>
-  <si>
     <t>USB-C</t>
   </si>
   <si>
@@ -210,6 +195,69 @@
   </si>
   <si>
     <t>USB-C CC resistors</t>
+  </si>
+  <si>
+    <t>Voltage regulator to limit VDD to 5V</t>
+  </si>
+  <si>
+    <t>TPS66121</t>
+  </si>
+  <si>
+    <t>296-TPS66121YBGRCT-ND</t>
+  </si>
+  <si>
+    <t>VDD coupling capacitor</t>
+  </si>
+  <si>
+    <t>VLDO coupling capacitor</t>
+  </si>
+  <si>
+    <t>VDD Schottky diode for reverse voltage protection</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>OVP voltage dividing resistor</t>
+  </si>
+  <si>
+    <t>102k</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>D257</t>
+  </si>
+  <si>
+    <t>C258</t>
+  </si>
+  <si>
+    <t>C257</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>4.7u</t>
+  </si>
+  <si>
+    <t>MBR230S1F-7</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>MBR230S1F-7DICT-ND</t>
+  </si>
+  <si>
+    <t>SOD123F</t>
+  </si>
+  <si>
+    <t>Pkg</t>
   </si>
 </sst>
 </file>
@@ -354,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -416,35 +464,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -761,37 +797,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD9514A-9B29-435C-BF48-54525C97080F}">
-  <dimension ref="B2:N12"/>
+  <dimension ref="B2:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.81640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.81640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.6328125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:14" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" ht="64" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -802,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>2</v>
@@ -811,7 +847,7 @@
         <v>22</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>5</v>
@@ -823,16 +859,16 @@
         <v>7</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
@@ -843,14 +879,14 @@
         <v>256</v>
       </c>
       <c r="E4" s="11">
-        <f t="shared" ref="E4:E11" si="0">D4*$C$2</f>
+        <f t="shared" ref="E4:E16" si="0">D4*$C$2</f>
         <v>768</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
@@ -863,7 +899,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="L4" s="5">
-        <f t="shared" ref="L4:L11" si="1">D4*K4</f>
+        <f t="shared" ref="L4:L16" si="1">D4*K4</f>
         <v>148.47999999999999</v>
       </c>
       <c r="M4" s="5">
@@ -871,10 +907,10 @@
         <v>445.43999999999994</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" ht="32" x14ac:dyDescent="0.2">
       <c r="B5" s="13" t="s">
         <v>21</v>
       </c>
@@ -892,16 +928,16 @@
         <v>20</v>
       </c>
       <c r="G5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="K5" s="2">
         <v>0.1</v>
@@ -911,14 +947,14 @@
         <v>25.6</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" ref="M5:M11" si="2">K5*E5</f>
+        <f t="shared" ref="M5:M16" si="2">K5*E5</f>
         <v>76.800000000000011</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
@@ -936,7 +972,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
@@ -957,12 +993,12 @@
         <v>1.56</v>
       </c>
       <c r="N6" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:14" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="13" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -975,25 +1011,25 @@
         <v>3</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="K7" s="2">
         <v>0.51</v>
       </c>
-      <c r="L7" s="2">
-        <f>K7*D7</f>
+      <c r="L7" s="26">
+        <f t="shared" si="1"/>
         <v>0.51</v>
       </c>
       <c r="M7" s="2">
@@ -1001,193 +1037,373 @@
         <v>1.53</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="B8" s="16" t="s">
+    <row r="8" spans="2:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="13"/>
+      <c r="C8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" ref="E8:E12" si="3">D8*$C$2</f>
+        <v>3</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" ref="M8:M12" si="4">K8*E8</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" spans="2:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="13"/>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="2:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="B10" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.41</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="2"/>
+        <v>1.23</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="B11" s="13"/>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="15"/>
+    </row>
+    <row r="12" spans="2:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="B12" s="13"/>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="15"/>
+    </row>
+    <row r="13" spans="2:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="B13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="17">
+        <v>1</v>
+      </c>
+      <c r="E13" s="17">
+        <f t="shared" ref="E13:E14" si="5">D13*$C$2</f>
+        <v>3</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="6">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" ref="L13" si="6">K13*D13</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="M13" s="6">
+        <f t="shared" ref="M13:M14" si="7">K13*E13</f>
+        <v>3.4799999999999995</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="B14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="H14" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="17">
+      <c r="I14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="L14" s="2">
+        <f>K14*D14</f>
+        <v>0.46</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="7"/>
+        <v>1.3800000000000001</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="16">
+        <v>22122044</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="17">
         <v>1</v>
       </c>
-      <c r="E8" s="17">
-        <f t="shared" ref="E8:E9" si="3">D8*$C$2</f>
-        <v>3</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="L8" s="6">
-        <f t="shared" ref="L8" si="4">K8*D8</f>
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="M8" s="6">
-        <f t="shared" ref="M8:M9" si="5">K8*E8</f>
-        <v>3.4799999999999995</v>
-      </c>
-      <c r="N8" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="21">
-        <v>2</v>
-      </c>
-      <c r="E9" s="21">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="24">
-        <v>0.23</v>
-      </c>
-      <c r="L9" s="24">
-        <f>K9*D9</f>
-        <v>0.46</v>
-      </c>
-      <c r="M9" s="24">
-        <f t="shared" si="5"/>
-        <v>1.3800000000000001</v>
-      </c>
-      <c r="N9" s="25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="16">
-        <v>22122044</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="17">
-        <v>1</v>
-      </c>
-      <c r="E10" s="17">
+      <c r="E15" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" s="6">
+      <c r="F15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="6">
         <v>1.28</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L15" s="6">
         <f t="shared" si="1"/>
         <v>1.28</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M15" s="6">
         <f t="shared" si="2"/>
         <v>3.84</v>
       </c>
-      <c r="N10" s="18" t="s">
-        <v>41</v>
+      <c r="N15" s="18" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="26">
+    <row r="16" spans="2:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="B16" s="21">
         <v>2177961041</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="27">
+      <c r="C16" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="22">
         <v>1</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E16" s="22">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F11" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="28" t="s">
+      <c r="F16" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="J16" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="29">
+      <c r="K16" s="24">
         <v>2.87</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L16" s="24">
         <f t="shared" si="1"/>
         <v>2.87</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M16" s="24">
         <f t="shared" si="2"/>
         <v>8.61</v>
       </c>
-      <c r="N11" s="30" t="s">
-        <v>41</v>
+      <c r="N16" s="25" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="L12" s="2">
-        <f>SUM(L4:L11)</f>
-        <v>180.88</v>
-      </c>
-      <c r="M12" s="2">
-        <f>L12*$C$2</f>
-        <v>542.64</v>
+    <row r="17" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L17" s="2">
+        <f>SUM(L4:L16)</f>
+        <v>181.29</v>
+      </c>
+      <c r="M17" s="2">
+        <f>L17*$C$2</f>
+        <v>543.87</v>
       </c>
     </row>
   </sheetData>
@@ -1196,31 +1412,32 @@
     <hyperlink ref="B4" r:id="rId1" xr:uid="{3A0E0B2C-17EE-3D41-96E9-F139CB8A2E54}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{9999CBF9-0CDD-4B48-B955-7479237F2071}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{6D999CED-9711-4640-A005-827337416F33}"/>
-    <hyperlink ref="B10" r:id="rId4" display="https://www.digikey.com/en/products/detail/molex/0022122044/172037?s=N4IgTCBcDaIOoFkwHYCMBmAtAOQCIgF0BfIA" xr:uid="{7437B1C3-056F-0144-ABD4-205DC0CF3893}"/>
-    <hyperlink ref="B11" r:id="rId5" display="https://www.digikey.com/en/products/detail/molex/2177961041/14638035?s=N4IgTCBcDaIJwAYEFowEYDsG4DY0IBY1kA5AERAF0BfIA" xr:uid="{D06D4DCF-3FAD-A643-A76D-087102DD2020}"/>
+    <hyperlink ref="B15" r:id="rId4" display="https://www.digikey.com/en/products/detail/molex/0022122044/172037?s=N4IgTCBcDaIOoFkwHYCMBmAtAOQCIgF0BfIA" xr:uid="{7437B1C3-056F-0144-ABD4-205DC0CF3893}"/>
+    <hyperlink ref="B16" r:id="rId5" display="https://www.digikey.com/en/products/detail/molex/2177961041/14638035?s=N4IgTCBcDaIJwAYEFowEYDsG4DY0IBY1kA5AERAF0BfIA" xr:uid="{D06D4DCF-3FAD-A643-A76D-087102DD2020}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{9592E701-99FA-1B45-BF3D-975C7A1DA5D3}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{E2A5498C-D55C-FA4D-B8F4-F48B72971313}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{6AE1B05E-E8D8-4CC5-93EF-48089028ABE7}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{E2A5498C-D55C-FA4D-B8F4-F48B72971313}"/>
+    <hyperlink ref="B14" r:id="rId8" xr:uid="{6AE1B05E-E8D8-4CC5-93EF-48089028ABE7}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{2F0245ED-1BC6-BF4D-9543-C9F818E0783D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ba1fd6c3-18a5-4ad5-8874-cc8651459af8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ba1fd6c3-18a5-4ad5-8874-cc8651459af8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1445,14 +1662,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23CEE53E-8C79-44C3-9A5B-668821A655FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B49F70-5F7A-4E2F-80DA-5D6488B232AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1465,6 +1674,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="ba1fd6c3-18a5-4ad5-8874-cc8651459af8"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23CEE53E-8C79-44C3-9A5B-668821A655FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
finished BOm for v2
</commit_message>
<xml_diff>
--- a/Hardware/LED_Matrix_2-0_BOM.xlsx
+++ b/Hardware/LED_Matrix_2-0_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eleanortaylor/Documents/GitHub/LED_Matrix/Hardware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etaylor\Documents\LED_Matrix\LED_Matrix\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CF33BE-6A15-0145-855F-1A42D7D4D261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAED8D3-4E58-47C8-88E1-132022550FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CBCE60BC-0067-4A82-873C-C47F583079C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CBCE60BC-0067-4A82-873C-C47F583079C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
   <si>
     <t>Part number</t>
   </si>
@@ -110,9 +110,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>100nF</t>
-  </si>
-  <si>
     <t>Kyocera</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>Rx</t>
   </si>
   <si>
-    <t>5.1kOhm</t>
-  </si>
-  <si>
     <t>Vishay Dale</t>
   </si>
   <si>
@@ -257,7 +251,49 @@
     <t>SOD123F</t>
   </si>
   <si>
-    <t>Pkg</t>
+    <t>C0805C106J8RACAUTO7210</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>399-C0805C106J8RACAUTO7210CT-ND</t>
+  </si>
+  <si>
+    <t>399-15708-1-ND</t>
+  </si>
+  <si>
+    <t>C0805C475J8RACAUTO</t>
+  </si>
+  <si>
+    <t>ERJ-PB6D2002V</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>P21165CT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-PB6B1023V</t>
+  </si>
+  <si>
+    <t>P20823CT-ND</t>
+  </si>
+  <si>
+    <t>Pkg.</t>
+  </si>
+  <si>
+    <t>5.1k</t>
+  </si>
+  <si>
+    <t>100n</t>
+  </si>
+  <si>
+    <t>14-SOIC</t>
+  </si>
+  <si>
+    <t>28-DSBGA</t>
   </si>
 </sst>
 </file>
@@ -402,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -464,23 +500,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -799,35 +847,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD9514A-9B29-435C-BF48-54525C97080F}">
   <dimension ref="B2:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.83203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14" ht="60" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -838,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>2</v>
@@ -847,7 +892,7 @@
         <v>22</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>5</v>
@@ -859,16 +904,16 @@
         <v>7</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
@@ -888,7 +933,9 @@
       <c r="G4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="I4" s="7" t="s">
         <v>11</v>
       </c>
@@ -896,21 +943,21 @@
         <v>12</v>
       </c>
       <c r="K4" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" ref="L4:L16" si="1">D4*K4</f>
-        <v>148.47999999999999</v>
+        <v>153.6</v>
       </c>
       <c r="M4" s="5">
         <f>K4*E4</f>
-        <v>445.43999999999994</v>
+        <v>460.79999999999995</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>21</v>
       </c>
@@ -928,16 +975,16 @@
         <v>20</v>
       </c>
       <c r="G5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="K5" s="2">
         <v>0.1</v>
@@ -951,10 +998,10 @@
         <v>76.800000000000011</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
@@ -974,7 +1021,9 @@
       <c r="G6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="I6" s="9" t="s">
         <v>17</v>
       </c>
@@ -982,23 +1031,23 @@
         <v>16</v>
       </c>
       <c r="K6" s="6">
-        <v>0.52</v>
+        <v>0.38</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" si="1"/>
-        <v>0.52</v>
+        <v>0.38</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" si="2"/>
-        <v>1.56</v>
+        <v>1.1400000000000001</v>
       </c>
       <c r="N6" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -1011,73 +1060,85 @@
         <v>3</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>17</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K7" s="2">
-        <v>0.51</v>
-      </c>
-      <c r="L7" s="26">
+        <v>1</v>
+      </c>
+      <c r="L7" s="21">
         <f t="shared" si="1"/>
-        <v>0.51</v>
+        <v>1</v>
       </c>
       <c r="M7" s="2">
         <f>K7*E7</f>
-        <v>1.53</v>
+        <v>3</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="13"/>
-      <c r="C8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="1">
+    <row r="8" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="17">
         <v>1</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="17">
         <f t="shared" ref="E8:E12" si="3">D8*$C$2</f>
         <v>3</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2">
+      <c r="F8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="L8" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="2">
-        <f t="shared" ref="M8:M12" si="4">K8*E8</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="15"/>
+        <v>0.81</v>
+      </c>
+      <c r="M8" s="6">
+        <f t="shared" ref="M8" si="4">K8*E8</f>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="9" spans="2:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="13"/>
+    <row r="9" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1087,75 +1148,85 @@
         <v>3</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.53</v>
+      </c>
       <c r="L9" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N9" s="15"/>
+        <v>1.59</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="10" spans="2:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="B10" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="1">
+    <row r="10" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="17">
         <v>1</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="17">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="F10" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" s="8" t="s">
+      <c r="H10" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="K10" s="2">
+      <c r="I10" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="6">
         <v>0.41</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="6">
         <f t="shared" si="1"/>
         <v>0.41</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="6">
         <f t="shared" si="2"/>
         <v>1.23</v>
       </c>
-      <c r="N10" s="15" t="s">
-        <v>40</v>
+      <c r="N10" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="B11" s="13"/>
+    <row r="11" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -1165,245 +1236,263 @@
         <v>3</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.36</v>
+      </c>
       <c r="L11" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="15"/>
+        <v>1.08</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="12" spans="2:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="B12" s="13"/>
-      <c r="C12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="1">
+    <row r="12" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="17">
         <v>1</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="17">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2">
+      <c r="H12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="L12" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="M12" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="15"/>
+        <v>0.75</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="13" spans="2:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="B13" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="17">
+    <row r="13" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="27">
         <v>1</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="27">
         <f t="shared" ref="E13:E14" si="5">D13*$C$2</f>
         <v>3</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="9" t="s">
+      <c r="F13" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="9" t="s">
+      <c r="H13" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="K13" s="6">
+      <c r="K13" s="21">
         <v>1.1599999999999999</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="21">
         <f t="shared" ref="L13" si="6">K13*D13</f>
         <v>1.1599999999999999</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="21">
         <f t="shared" ref="M13:M14" si="7">K13*E13</f>
         <v>3.4799999999999995</v>
       </c>
-      <c r="N13" s="18" t="s">
-        <v>40</v>
+      <c r="N13" s="30" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="14" spans="2:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="B14" s="20" t="s">
+    <row r="14" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="D14" s="17">
         <v>2</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="17">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="F14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="K14" s="2">
+      <c r="K14" s="6">
         <v>0.23</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="6">
         <f>K14*D14</f>
         <v>0.46</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="6">
         <f t="shared" si="7"/>
         <v>1.3800000000000001</v>
       </c>
-      <c r="N14" s="15" t="s">
-        <v>40</v>
+      <c r="N14" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="16">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="20">
         <v>22122044</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="17">
+      <c r="C15" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="27">
         <v>1</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="27">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="9" t="s">
+      <c r="F15" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="K15" s="6">
+      <c r="I15" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" s="21">
         <v>1.28</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="21">
         <f t="shared" si="1"/>
         <v>1.28</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="21">
         <f t="shared" si="2"/>
         <v>3.84</v>
       </c>
-      <c r="N15" s="18" t="s">
-        <v>40</v>
+      <c r="N15" s="30" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="B16" s="21">
+    <row r="16" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="22">
         <v>2177961041</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="22">
+      <c r="C16" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="23">
         <v>1</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="23">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F16" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="23" t="s">
+      <c r="F16" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="H16" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="J16" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="K16" s="24">
+      <c r="K16" s="25">
         <v>2.87</v>
       </c>
-      <c r="L16" s="24">
+      <c r="L16" s="25">
         <f t="shared" si="1"/>
         <v>2.87</v>
       </c>
-      <c r="M16" s="24">
+      <c r="M16" s="25">
         <f t="shared" si="2"/>
         <v>8.61</v>
       </c>
-      <c r="N16" s="25" t="s">
-        <v>40</v>
+      <c r="N16" s="26" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="17" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L17" s="2">
         <f>SUM(L4:L16)</f>
-        <v>181.29</v>
+        <v>188.71</v>
       </c>
       <c r="M17" s="2">
         <f>L17*$C$2</f>
-        <v>543.87</v>
+        <v>566.13</v>
       </c>
     </row>
   </sheetData>
@@ -1418,29 +1507,17 @@
     <hyperlink ref="B13" r:id="rId7" xr:uid="{E2A5498C-D55C-FA4D-B8F4-F48B72971313}"/>
     <hyperlink ref="B14" r:id="rId8" xr:uid="{6AE1B05E-E8D8-4CC5-93EF-48089028ABE7}"/>
     <hyperlink ref="B10" r:id="rId9" xr:uid="{2F0245ED-1BC6-BF4D-9543-C9F818E0783D}"/>
+    <hyperlink ref="B8" r:id="rId10" xr:uid="{5CB6D934-AF60-4EB4-918D-D39F2CF68B0F}"/>
+    <hyperlink ref="B9" r:id="rId11" xr:uid="{24AA6C26-7C08-4183-8CD6-BFAF9CE8BEBC}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{5983D0DA-68FC-482D-A683-304602BA1983}"/>
+    <hyperlink ref="B11" r:id="rId13" xr:uid="{1918AFB2-D635-4DBB-BE88-19583627C766}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId14"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ba1fd6c3-18a5-4ad5-8874-cc8651459af8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100502A07BBE43C3E4CA597A0A715DE62F0" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ef1ef2518dbd8baba4018934b602a0f9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ba1fd6c3-18a5-4ad5-8874-cc8651459af8" xmlns:ns4="a68b5875-a714-48fe-ba43-532dbf3c5e2c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="47a0e7dd0dc87d993f33ac560f56e359" ns3:_="" ns4:_="">
     <xsd:import namespace="ba1fd6c3-18a5-4ad5-8874-cc8651459af8"/>
@@ -1661,32 +1738,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B49F70-5F7A-4E2F-80DA-5D6488B232AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="a68b5875-a714-48fe-ba43-532dbf3c5e2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ba1fd6c3-18a5-4ad5-8874-cc8651459af8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23CEE53E-8C79-44C3-9A5B-668821A655FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ba1fd6c3-18a5-4ad5-8874-cc8651459af8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EE7C584-7962-4C7B-8A56-C0162DDCE136}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1703,4 +1772,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23CEE53E-8C79-44C3-9A5B-668821A655FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B49F70-5F7A-4E2F-80DA-5D6488B232AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="a68b5875-a714-48fe-ba43-532dbf3c5e2c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ba1fd6c3-18a5-4ad5-8874-cc8651459af8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>